<commit_message>
Added comments to Averager.
</commit_message>
<xml_diff>
--- a/Non_Coding/pecuniary.xlsx
+++ b/Non_Coding/pecuniary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias\Documents\Programming\GitHub\MiscRep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias\Documents\Programming\GitHub\MiscRep\Non_Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>After Spending</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>Misc</t>
+  </si>
+  <si>
+    <t>Check 7/7/16</t>
+  </si>
+  <si>
+    <t>Café Espresso</t>
   </si>
 </sst>
 </file>
@@ -461,7 +467,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,31 +507,31 @@
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>H2*0.1</f>
-        <v>122.33800000000002</v>
+        <v>152.35600000000002</v>
       </c>
       <c r="B2" s="3">
         <f>H2*0.25</f>
-        <v>305.84500000000003</v>
+        <v>380.89000000000004</v>
       </c>
       <c r="C2" s="3">
         <f>H2*0.1</f>
-        <v>122.33800000000002</v>
+        <v>152.35600000000002</v>
       </c>
       <c r="D2" s="3">
-        <f>H2 * 0.35</f>
-        <v>428.18299999999999</v>
+        <f>H2 * 0.3</f>
+        <v>457.06800000000004</v>
       </c>
       <c r="E2" s="3">
         <f xml:space="preserve"> H2*0.1</f>
-        <v>122.33800000000002</v>
+        <v>152.35600000000002</v>
       </c>
       <c r="F2" s="3">
-        <f>H2*0.1</f>
-        <v>122.33800000000002</v>
+        <f>H2*0.15</f>
+        <v>228.53400000000002</v>
       </c>
       <c r="H2" s="3">
         <f>SUMPRODUCT(H7:H53,MOD(ROW(H7:H53)+1,2))</f>
-        <v>1223.3800000000001</v>
+        <v>1523.5600000000002</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
@@ -559,32 +565,32 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>SUMPRODUCT(A7:A53,MOD(ROW(A7:A53)+1,2))</f>
+        <f t="shared" ref="A4:F4" si="0">SUMPRODUCT(A7:A53,MOD(ROW(A7:A53)+1,2))</f>
         <v>32.58</v>
       </c>
       <c r="B4">
-        <f>SUMPRODUCT(B7:B53,MOD(ROW(B7:B53)+1,2))</f>
+        <f t="shared" si="0"/>
         <v>131.99</v>
       </c>
       <c r="C4" s="4">
-        <f>SUMPRODUCT(C7:C53,MOD(ROW(C7:C53)+1,2))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D4" s="4">
-        <f>SUMPRODUCT(D7:D53,MOD(ROW(D7:D53)+1,2))</f>
+        <f t="shared" si="0"/>
         <v>141.18</v>
       </c>
       <c r="E4">
-        <f>SUMPRODUCT(E7:E53,MOD(ROW(E7:E53)+1,2))</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>19.71</v>
       </c>
       <c r="F4">
-        <f>SUMPRODUCT(F7:F53,MOD(ROW(F7:F53)+1,2))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4">
         <f xml:space="preserve"> SUM(A4:G4)</f>
-        <v>305.75</v>
+        <v>325.45999999999998</v>
       </c>
       <c r="L4">
         <v>2336</v>
@@ -592,32 +598,32 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
-        <f>A2-A4</f>
-        <v>89.758000000000024</v>
+        <f t="shared" ref="A5:F5" si="1">A2-A4</f>
+        <v>119.77600000000002</v>
       </c>
       <c r="B5" s="4">
-        <f>B2-B4</f>
-        <v>173.85500000000002</v>
+        <f t="shared" si="1"/>
+        <v>248.90000000000003</v>
       </c>
       <c r="C5" s="4">
-        <f>C2-C4</f>
-        <v>122.33800000000002</v>
+        <f t="shared" si="1"/>
+        <v>152.35600000000002</v>
       </c>
       <c r="D5" s="4">
-        <f>D2-D4</f>
-        <v>287.00299999999999</v>
+        <f t="shared" si="1"/>
+        <v>315.88800000000003</v>
       </c>
       <c r="E5" s="4">
-        <f>E2-E4</f>
-        <v>122.33800000000002</v>
+        <f t="shared" si="1"/>
+        <v>132.64600000000002</v>
       </c>
       <c r="F5" s="4">
-        <f>F2-F4</f>
-        <v>122.33800000000002</v>
+        <f t="shared" si="1"/>
+        <v>228.53400000000002</v>
       </c>
       <c r="H5" s="7">
         <f>H2 - H4</f>
-        <v>917.63000000000011</v>
+        <v>1198.1000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -650,6 +656,9 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
@@ -664,6 +673,9 @@
       <c r="D8">
         <v>141.18</v>
       </c>
+      <c r="E8">
+        <v>19.71</v>
+      </c>
       <c r="H8">
         <v>719.85</v>
       </c>
@@ -690,9 +702,15 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
+      <c r="H14">
+        <v>300.18</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>

</xml_diff>

<commit_message>
Updated budget and added some missed files
</commit_message>
<xml_diff>
--- a/Non_Coding/pecuniary.xlsx
+++ b/Non_Coding/pecuniary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>After Spending</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Café Espresso</t>
+  </si>
+  <si>
+    <t>Phone Case</t>
+  </si>
+  <si>
+    <t>New Clothes</t>
+  </si>
+  <si>
+    <t>Check 7/14/16</t>
   </si>
 </sst>
 </file>
@@ -467,7 +476,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,31 +516,31 @@
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>H2*0.1</f>
-        <v>152.35600000000002</v>
+        <v>177.64400000000001</v>
       </c>
       <c r="B2" s="3">
         <f>H2*0.25</f>
-        <v>380.89000000000004</v>
+        <v>444.11</v>
       </c>
       <c r="C2" s="3">
         <f>H2*0.1</f>
-        <v>152.35600000000002</v>
+        <v>177.64400000000001</v>
       </c>
       <c r="D2" s="3">
         <f>H2 * 0.3</f>
-        <v>457.06800000000004</v>
+        <v>532.93200000000002</v>
       </c>
       <c r="E2" s="3">
         <f xml:space="preserve"> H2*0.1</f>
-        <v>152.35600000000002</v>
+        <v>177.64400000000001</v>
       </c>
       <c r="F2" s="3">
         <f>H2*0.15</f>
-        <v>228.53400000000002</v>
+        <v>266.46600000000001</v>
       </c>
       <c r="H2" s="3">
         <f>SUMPRODUCT(H7:H53,MOD(ROW(H7:H53)+1,2))</f>
-        <v>1523.5600000000002</v>
+        <v>1776.44</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
@@ -570,7 +579,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>131.99</v>
+        <v>201.23000000000002</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="0"/>
@@ -586,11 +595,11 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>66.819999999999993</v>
       </c>
       <c r="H4">
         <f xml:space="preserve"> SUM(A4:G4)</f>
-        <v>325.45999999999998</v>
+        <v>461.52</v>
       </c>
       <c r="L4">
         <v>2336</v>
@@ -599,31 +608,31 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" ref="A5:F5" si="1">A2-A4</f>
-        <v>119.77600000000002</v>
+        <v>145.06400000000002</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="1"/>
-        <v>248.90000000000003</v>
+        <v>242.88</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>152.35600000000002</v>
+        <v>177.64400000000001</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>315.88800000000003</v>
+        <v>391.75200000000001</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>132.64600000000002</v>
+        <v>157.934</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>228.53400000000002</v>
+        <v>199.64600000000002</v>
       </c>
       <c r="H5" s="7">
         <f>H2 - H4</f>
-        <v>1198.1000000000001</v>
+        <v>1314.92</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -642,6 +651,9 @@
       <c r="E6" t="s">
         <v>12</v>
       </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
       <c r="H6" t="s">
         <v>7</v>
       </c>
@@ -659,6 +671,9 @@
       <c r="E7" t="s">
         <v>20</v>
       </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" t="s">
         <v>9</v>
       </c>
@@ -676,16 +691,25 @@
       <c r="E8">
         <v>19.71</v>
       </c>
+      <c r="F8">
+        <v>66.819999999999993</v>
+      </c>
       <c r="H8">
         <v>719.85</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
       <c r="H9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>69.239999999999995</v>
+      </c>
       <c r="H10">
         <v>247.56</v>
       </c>
@@ -714,9 +738,15 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
+      <c r="H16">
+        <v>252.88</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>

</xml_diff>

<commit_message>
Updating rep, including budget and therealpi.co.nf, to implement version control
</commit_message>
<xml_diff>
--- a/Non_Coding/pecuniary.xlsx
+++ b/Non_Coding/pecuniary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>After Spending</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Check 7/14/16</t>
+  </si>
+  <si>
+    <t>Check 7/21/16</t>
   </si>
 </sst>
 </file>
@@ -476,7 +479,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,31 +519,31 @@
     <row r="2" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <f>H2*0.1</f>
-        <v>177.64400000000001</v>
+        <v>201.88200000000003</v>
       </c>
       <c r="B2" s="3">
         <f>H2*0.25</f>
-        <v>444.11</v>
+        <v>504.70500000000004</v>
       </c>
       <c r="C2" s="3">
         <f>H2*0.1</f>
-        <v>177.64400000000001</v>
+        <v>201.88200000000003</v>
       </c>
       <c r="D2" s="3">
         <f>H2 * 0.3</f>
-        <v>532.93200000000002</v>
+        <v>605.64600000000007</v>
       </c>
       <c r="E2" s="3">
         <f xml:space="preserve"> H2*0.1</f>
-        <v>177.64400000000001</v>
+        <v>201.88200000000003</v>
       </c>
       <c r="F2" s="3">
         <f>H2*0.15</f>
-        <v>266.46600000000001</v>
+        <v>302.82300000000004</v>
       </c>
       <c r="H2" s="3">
         <f>SUMPRODUCT(H7:H53,MOD(ROW(H7:H53)+1,2))</f>
-        <v>1776.44</v>
+        <v>2018.8200000000002</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>10</v>
@@ -608,31 +611,31 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <f t="shared" ref="A5:F5" si="1">A2-A4</f>
-        <v>145.06400000000002</v>
+        <v>169.30200000000002</v>
       </c>
       <c r="B5" s="4">
         <f t="shared" si="1"/>
-        <v>242.88</v>
+        <v>303.47500000000002</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>177.64400000000001</v>
+        <v>201.88200000000003</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="1"/>
-        <v>391.75200000000001</v>
+        <v>464.46600000000007</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="1"/>
-        <v>157.934</v>
+        <v>182.17200000000003</v>
       </c>
       <c r="F5" s="4">
         <f t="shared" si="1"/>
-        <v>199.64600000000002</v>
+        <v>236.00300000000004</v>
       </c>
       <c r="H5" s="7">
         <f>H2 - H4</f>
-        <v>1314.92</v>
+        <v>1557.3000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -748,17 +751,23 @@
         <v>252.88</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="2:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>242.38</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
     </row>
   </sheetData>

</xml_diff>